<commit_message>
Updated datasets to reflect changes to database
</commit_message>
<xml_diff>
--- a/database/test-import-data/students/data.xlsx
+++ b/database/test-import-data/students/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saahi\OneDrive\Desktop\overseas-travel-database-management-system\database\test-import-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saahi\OneDrive\Desktop\overseas-travel-database-management-system\database\test-import-data\students\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F76DAEA5-95DA-45EE-8B03-7240E5A2208D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBBE0C53-52A3-4216-BC9A-C6DFDF21A326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{06BB8B05-F846-4CCD-AA37-3D2CA17146F6}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{06BB8B05-F846-4CCD-AA37-3D2CA17146F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,26 +44,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>adminNo</t>
   </si>
   <si>
-    <t>gender</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
     <t>citizenshipStatus</t>
   </si>
   <si>
-    <t>course</t>
-  </si>
-  <si>
-    <t>stage</t>
-  </si>
-  <si>
     <t>pemGroup</t>
   </si>
   <si>
@@ -73,18 +64,6 @@
     <t>XLSX Uno</t>
   </si>
   <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>Singapore citizen</t>
-  </si>
-  <si>
-    <t>C02</t>
-  </si>
-  <si>
-    <t>MI2002</t>
-  </si>
-  <si>
     <t>212346A</t>
   </si>
   <si>
@@ -95,6 +74,21 @@
   </si>
   <si>
     <t>XLSX Tres</t>
+  </si>
+  <si>
+    <t>studyStage</t>
+  </si>
+  <si>
+    <t>courseCode</t>
+  </si>
+  <si>
+    <t>Singapore Citizen</t>
+  </si>
+  <si>
+    <t>EGDF21</t>
+  </si>
+  <si>
+    <t>IM2000</t>
   </si>
 </sst>
 </file>
@@ -479,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CB91F20-FB48-493B-927B-380DE584D14D}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -491,100 +485,89 @@
     <col min="7" max="7" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2">
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="E4" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="F4" t="s">
         <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>